<commit_message>
Docs update to match new sections implementation
</commit_message>
<xml_diff>
--- a/docs/distrib.xlsx
+++ b/docs/distrib.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammed Ehab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\learning\distributed\OpenMP Codon Frequency\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9C8BFA-DB35-4A01-A1BA-EA619FCCAE73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD802F0A-A98E-4385-B0E8-D5BBB1287303}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{4E395B02-0435-48AB-AD0A-878D34393581}"/>
   </bookViews>
@@ -209,16 +209,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>244</c:v>
+                  <c:v>248</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>234</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>240</c:v>
+                  <c:v>232</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>257</c:v>
+                  <c:v>233</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -296,16 +296,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>185</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>126</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>139</c:v>
+                  <c:v>157</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1518,8 +1518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A53BF75-6442-4B9C-A0A6-243CF8E8CACB}">
   <dimension ref="A2:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1562,76 +1562,76 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
-        <v>341</v>
+      <c r="B4" s="1">
+        <v>366</v>
       </c>
       <c r="C4" s="1">
-        <v>185</v>
+        <v>204</v>
       </c>
       <c r="D4" s="2">
         <f>B4/C4</f>
-        <v>1.8432432432432433</v>
+        <v>1.7941176470588236</v>
       </c>
       <c r="E4" s="1">
         <f>D4/A4</f>
-        <v>0.92162162162162165</v>
+        <v>0.8970588235294118</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
-        <v>295</v>
+      <c r="B5" s="1">
+        <v>238</v>
       </c>
       <c r="C5" s="1">
         <v>117</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" ref="D5:D7" si="0">B5/C5</f>
-        <v>2.5213675213675213</v>
+        <v>2.0341880341880341</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" ref="E5:E7" si="1">D5/A5</f>
-        <v>0.63034188034188032</v>
+        <v>0.50854700854700852</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>8</v>
       </c>
-      <c r="B6" s="2">
-        <v>242</v>
+      <c r="B6" s="1">
+        <v>239</v>
       </c>
       <c r="C6" s="1">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>1.9206349206349207</v>
+        <v>1.9274193548387097</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="1"/>
-        <v>0.24007936507936509</v>
+        <v>0.24092741935483872</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>16</v>
       </c>
-      <c r="B7" s="2">
-        <v>244</v>
+      <c r="B7" s="1">
+        <v>241</v>
       </c>
       <c r="C7" s="1">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>1.7553956834532374</v>
+        <v>1.5350318471337581</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="1"/>
-        <v>0.10971223021582734</v>
+        <v>9.5939490445859879E-2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -1644,19 +1644,19 @@
       </c>
       <c r="B9" s="2">
         <f>SUM(B4:B7)/4</f>
-        <v>280.5</v>
+        <v>271</v>
       </c>
       <c r="C9" s="2">
         <f>SUM(C4:C7)/4</f>
-        <v>141.75</v>
+        <v>150.5</v>
       </c>
       <c r="D9" s="2">
         <f>SUM(D4:D7)/4</f>
-        <v>2.0101603421747307</v>
+        <v>1.8226892208048313</v>
       </c>
       <c r="E9" s="1">
         <f>SUM(E4:E7)/4</f>
-        <v>0.47543877431467363</v>
+        <v>0.43561818546927972</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1688,76 +1688,76 @@
       <c r="A14" s="1">
         <v>2</v>
       </c>
-      <c r="B14" s="2">
-        <v>341</v>
+      <c r="B14" s="1">
+        <v>366</v>
       </c>
       <c r="C14" s="1">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D14" s="2">
         <f>B14/C14</f>
-        <v>1.3975409836065573</v>
+        <v>1.4758064516129032</v>
       </c>
       <c r="E14" s="1">
         <f>D14/A14</f>
-        <v>0.69877049180327866</v>
+        <v>0.73790322580645162</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>4</v>
       </c>
-      <c r="B15" s="2">
-        <v>295</v>
+      <c r="B15" s="1">
+        <v>238</v>
       </c>
       <c r="C15" s="1">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" ref="D15:D17" si="2">B15/C15</f>
-        <v>1.2606837606837606</v>
+        <v>1.1069767441860465</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" ref="E15:E17" si="3">D15/A15</f>
-        <v>0.31517094017094016</v>
+        <v>0.27674418604651163</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>8</v>
       </c>
-      <c r="B16" s="2">
-        <v>242</v>
+      <c r="B16" s="1">
+        <v>239</v>
       </c>
       <c r="C16" s="1">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="2"/>
-        <v>1.0083333333333333</v>
+        <v>1.0301724137931034</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="3"/>
-        <v>0.12604166666666666</v>
+        <v>0.12877155172413793</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="2">
-        <v>244</v>
+      <c r="B17" s="1">
+        <v>241</v>
       </c>
       <c r="C17" s="1">
-        <v>257</v>
+        <v>233</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="2"/>
-        <v>0.94941634241245132</v>
+        <v>1.0343347639484979</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="3"/>
-        <v>5.9338521400778207E-2</v>
+        <v>6.4645922746781118E-2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -1770,19 +1770,19 @@
       </c>
       <c r="B19" s="2">
         <f>SUM(B14:B17)/4</f>
-        <v>280.5</v>
+        <v>271</v>
       </c>
       <c r="C19" s="2">
         <f>SUM(C14:C17)/4</f>
-        <v>243.75</v>
+        <v>232</v>
       </c>
       <c r="D19" s="2">
         <f>SUM(D14:D17)/4</f>
-        <v>1.1539936050090256</v>
+        <v>1.1618225933851376</v>
       </c>
       <c r="E19" s="1">
         <f>SUM(E14:E17)/4</f>
-        <v>0.29983040501041591</v>
+        <v>0.30201622158097058</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="58" x14ac:dyDescent="0.35">
@@ -1809,13 +1809,13 @@
         <v>2</v>
       </c>
       <c r="B24" s="1">
-        <v>341</v>
+        <v>366</v>
       </c>
       <c r="C24" s="1">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D24" s="1">
-        <v>185</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1823,10 +1823,10 @@
         <v>4</v>
       </c>
       <c r="B25" s="1">
-        <v>295</v>
+        <v>238</v>
       </c>
       <c r="C25" s="1">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="D25" s="1">
         <v>117</v>
@@ -1837,13 +1837,13 @@
         <v>8</v>
       </c>
       <c r="B26" s="1">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C26" s="1">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="D26" s="1">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -1851,13 +1851,13 @@
         <v>16</v>
       </c>
       <c r="B27" s="1">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C27" s="1">
-        <v>257</v>
+        <v>233</v>
       </c>
       <c r="D27" s="1">
-        <v>139</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1866,15 +1866,15 @@
       </c>
       <c r="B29" s="2">
         <f>SUM(B24:B27)/4</f>
-        <v>280.5</v>
+        <v>271</v>
       </c>
       <c r="C29" s="2">
         <f>SUM(C24:C27)/4</f>
-        <v>243.75</v>
+        <v>232</v>
       </c>
       <c r="D29" s="2">
         <f>SUM(D24:D27)/4</f>
-        <v>141.75</v>
+        <v>150.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>